<commit_message>
Add spreadsheet with benchmarking results
</commit_message>
<xml_diff>
--- a/benchmarking/results.xlsx
+++ b/benchmarking/results.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/luiz_fonseca_ulb_be/Documents/Database Systems Architecture/project/benchmarking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_AD4D361C20488DEA4E38A02FC4D951765ADEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1EDACCC-1CDF-4EF2-BA21-2240A07AF828}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_AD4D361C20488DEA4E38A02FC4D951765ADEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A77E35F-7E39-4F17-A0C7-6BEE59069F3E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>benchmarking-goal</t>
   </si>
@@ -40,14 +49,84 @@
   </si>
   <si>
     <t>actual-result</t>
+  </si>
+  <si>
+    <t>compare distributions</t>
+  </si>
+  <si>
+    <t>normal-normal</t>
+  </si>
+  <si>
+    <t>normal-left</t>
+  </si>
+  <si>
+    <t>normal-right</t>
+  </si>
+  <si>
+    <t>left-left</t>
+  </si>
+  <si>
+    <t>left-right</t>
+  </si>
+  <si>
+    <t>right-right</t>
+  </si>
+  <si>
+    <t>compare table size</t>
+  </si>
+  <si>
+    <t>small-small</t>
+  </si>
+  <si>
+    <t>small-big</t>
+  </si>
+  <si>
+    <t>big-big</t>
+  </si>
+  <si>
+    <t>compare range size</t>
+  </si>
+  <si>
+    <t>compare range type</t>
+  </si>
+  <si>
+    <t>integer-integer</t>
+  </si>
+  <si>
+    <t>float-float</t>
+  </si>
+  <si>
+    <t>date-date</t>
+  </si>
+  <si>
+    <t>timestamp-timestamp</t>
+  </si>
+  <si>
+    <t>Error(%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,8 +154,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,39 +438,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>5000</v>
+      </c>
+      <c r="D2">
+        <v>632683</v>
+      </c>
+      <c r="E2">
+        <v>645720</v>
+      </c>
+      <c r="F2">
+        <f>ABS(D2-E2)/E2 * 100</f>
+        <v>2.0189865576410826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>5000</v>
+      </c>
+      <c r="D3">
+        <v>405548</v>
+      </c>
+      <c r="E3">
+        <v>412419</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F17" si="0">ABS(D3-E3)/E3 * 100</f>
+        <v>1.6660241162507063</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>5000</v>
+      </c>
+      <c r="D4">
+        <v>388295</v>
+      </c>
+      <c r="E4">
+        <v>395599</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1.8463140705613512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <v>277522</v>
+      </c>
+      <c r="E5">
+        <v>282579</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.7895880444052814</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>5000</v>
+      </c>
+      <c r="D6">
+        <v>123713</v>
+      </c>
+      <c r="E6">
+        <v>124635</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.73976009949051225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>5000</v>
+      </c>
+      <c r="D7">
+        <v>291540</v>
+      </c>
+      <c r="E7">
+        <v>296764</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.7603213327762126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>5000</v>
+      </c>
+      <c r="D8">
+        <v>632683</v>
+      </c>
+      <c r="E8">
+        <v>645720</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2.0189865576410826</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>50000</v>
+      </c>
+      <c r="D9">
+        <v>6465052</v>
+      </c>
+      <c r="E9">
+        <v>6595967</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1.9847734229113032</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>500000</v>
+      </c>
+      <c r="D10">
+        <v>65434760</v>
+      </c>
+      <c r="E10">
+        <v>66816631</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2.0681542593789262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>5000</v>
+      </c>
+      <c r="D11">
+        <v>632683</v>
+      </c>
+      <c r="E11">
+        <v>645720</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2.0189865576410826</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>5000</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>5000</v>
+      </c>
+      <c r="D13">
+        <v>659151</v>
+      </c>
+      <c r="E13">
+        <v>672777</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>2.0253367757815739</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>5000</v>
+      </c>
+      <c r="D14">
+        <v>632683</v>
+      </c>
+      <c r="E14">
+        <v>645720</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>2.0189865576410826</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>5000</v>
+      </c>
+      <c r="D15">
+        <v>669241</v>
+      </c>
+      <c r="E15">
+        <v>679658</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1.5326826139028746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>5000</v>
+      </c>
+      <c r="D16">
+        <v>647976</v>
+      </c>
+      <c r="E16">
+        <v>658641</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>1.6192432599853332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>5000</v>
+      </c>
+      <c r="D17">
+        <v>654936</v>
+      </c>
+      <c r="E17" s="2">
+        <v>668499</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>2.0288736407982659</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>